<commit_message>
Cambios del dia 6/5
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitedits-my.sharepoint.com/personal/alicia_lopez_united-its_com/Documents/Documentos/UiPath/MARK-DISPATCHER/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="14_{962AAB0B-76A8-464F-B409-3662FB7438A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15BD07DC-CC94-4870-B7C6-DCBB13C41C11}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="14_{962AAB0B-76A8-464F-B409-3662FB7438A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3DE2F0B-69BF-4258-B1D6-E32A4F958953}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>C:\Users\Alicia LV\OneDrive - united-its.com\Documentos\UiPath\MARK-DISPATCHER\Data\Clientes\</t>
+  </si>
+  <si>
+    <t>PathExcelFileFiltered</t>
+  </si>
+  <si>
+    <t>C:\Users\Alicia LV\OneDrive - united-its.com\Documentos\UiPath\MARK-DISPATCHER\Data\ClientesFiltrados\</t>
   </si>
 </sst>
 </file>
@@ -303,6 +309,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,16 +614,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="94.26953125" customWidth="1"/>
-    <col min="3" max="3" width="100.54296875" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" customWidth="1"/>
+    <col min="3" max="3" width="100.5703125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -661,7 +671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.5">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" s="5" t="s">
         <v>53</v>
       </c>
@@ -683,7 +693,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.5">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
@@ -774,8 +784,12 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="4"/>
@@ -1778,12 +1792,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1820,7 +1834,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1831,7 +1845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1945,7 +1959,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2941,13 +2955,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="26" width="65.453125" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Añadido los tres modulos del performer para enviar emails.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitedits-my.sharepoint.com/personal/alicia_lopez_united-its_com/Documents/Documentos/UiPath/UITS_09/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alicia LV\OneDrive - united-its.com\Documentos\UiPath\UITS_09\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{27F1A4C9-6C08-4874-AC64-05BF5F91E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5A2A08-45F0-4E1D-86BD-A290ED4E7719}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B34F17-E395-4FC9-9985-5BFEB0F8FBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,7 +201,7 @@
     <t>C:\Users\Alicia LV\OneDrive - united-its.com\Documentos\UiPath\UITS_09\Data\Clientes\</t>
   </si>
   <si>
-    <t>EXCEL;Chrome;</t>
+    <t>EXCEL;Chrome</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
performer con las excepciones añadidas y modificaciones para depurarlas
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alicia LV\OneDrive - united-its.com\Documentos\UiPath\UITS_09\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B34F17-E395-4FC9-9985-5BFEB0F8FBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEDE65B-1200-4D8E-86AA-B26C6851B709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>EXCEL;Chrome</t>
+  </si>
+  <si>
+    <t>Client Support Contact</t>
+  </si>
+  <si>
+    <t>alicia.lopez@united-its.com</t>
+  </si>
+  <si>
+    <t>Email del cliente al que enviar información relativa a las excepciones de negocio que puedan surgir a lo largo de la ejecución</t>
   </si>
 </sst>
 </file>
@@ -598,16 +607,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="94.26953125" customWidth="1"/>
-    <col min="3" max="3" width="100.54296875" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" customWidth="1"/>
+    <col min="3" max="3" width="110.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -655,7 +664,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.5">
+    <row r="3" spans="1:26">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -671,7 +680,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.5">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
@@ -753,7 +762,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -761,26 +770,39 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1752,9 +1774,10 @@
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{6B027BB6-6A13-485F-A6E7-F2202D182AC9}"/>
     <hyperlink ref="B9" r:id="rId2" xr:uid="{7C6D8180-64F7-4A92-9BD4-66A61AC65FFD}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{0B53CE07-CCEE-4997-9696-632FE3BC0858}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1766,12 +1789,12 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1808,7 +1831,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1819,7 +1842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1933,7 +1956,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2929,13 +2952,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="4" width="70" customWidth="1"/>
-    <col min="5" max="26" width="65.453125" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>